<commit_message>
Montando dataset completo a partir da planilha
</commit_message>
<xml_diff>
--- a/imagens selecionadas.xlsx
+++ b/imagens selecionadas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maril\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariliasi\Documents\neuralNetworkWithImagesCT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB28BAE-2974-4AC1-809B-DA245573113B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075"/>
   </bookViews>
   <sheets>
     <sheet name="Página1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="821" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="160">
   <si>
     <t>TCIA Number com polipo</t>
   </si>
@@ -505,7 +504,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -703,8 +702,36 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Vírgula" xfId="1" builtinId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1012,23 +1039,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="23.33203125" customWidth="1"/>
-    <col min="6" max="6" width="23.33203125" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="14" t="s">
         <v>0</v>
@@ -1050,7 +1077,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>6</v>
       </c>
@@ -1061,7 +1088,7 @@
         <v>148</v>
       </c>
       <c r="D2" s="1">
-        <f t="shared" ref="D2:D66" si="0">C2+1</f>
+        <f t="shared" ref="D2:D65" si="0">C2+1</f>
         <v>149</v>
       </c>
       <c r="E2" s="15" t="s">
@@ -1079,7 +1106,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="19"/>
       <c r="B3" s="3" t="s">
         <v>7</v>
@@ -1104,7 +1131,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="19"/>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -1129,7 +1156,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="19"/>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -1153,7 +1180,7 @@
         <v>087</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="19"/>
       <c r="B6" s="3" t="s">
         <v>14</v>
@@ -1178,7 +1205,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="19"/>
       <c r="B7" s="3" t="s">
         <v>16</v>
@@ -1203,7 +1230,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="19"/>
       <c r="B8" s="3" t="s">
         <v>16</v>
@@ -1228,7 +1255,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="19"/>
       <c r="B9" s="3" t="s">
         <v>19</v>
@@ -1253,7 +1280,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="19"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
@@ -1278,7 +1305,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="19"/>
       <c r="B11" s="3" t="s">
         <v>21</v>
@@ -1303,7 +1330,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="19"/>
       <c r="B12" s="3" t="s">
         <v>23</v>
@@ -1328,7 +1355,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="19"/>
       <c r="B13" s="3" t="s">
         <v>25</v>
@@ -1353,7 +1380,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="19"/>
       <c r="B14" s="3" t="s">
         <v>25</v>
@@ -1378,7 +1405,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="19"/>
       <c r="B15" s="3" t="s">
         <v>28</v>
@@ -1403,7 +1430,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="19"/>
       <c r="B16" s="3" t="s">
         <v>30</v>
@@ -1428,7 +1455,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="19"/>
       <c r="B17" s="3" t="s">
         <v>32</v>
@@ -1453,7 +1480,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="19"/>
       <c r="B18" s="3" t="s">
         <v>34</v>
@@ -1476,7 +1503,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="19"/>
       <c r="B19" s="3" t="s">
         <v>36</v>
@@ -1501,7 +1528,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="19"/>
       <c r="B20" s="3" t="s">
         <v>36</v>
@@ -1526,7 +1553,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="19"/>
       <c r="B21" s="3" t="s">
         <v>36</v>
@@ -1550,7 +1577,7 @@
         <v>075</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="19"/>
       <c r="B22" s="3" t="s">
         <v>40</v>
@@ -1575,7 +1602,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="19"/>
       <c r="B23" s="3" t="s">
         <v>40</v>
@@ -1600,7 +1627,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="19"/>
       <c r="B24" s="3" t="s">
         <v>43</v>
@@ -1625,7 +1652,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="19"/>
       <c r="B25" s="3" t="s">
         <v>45</v>
@@ -1650,7 +1677,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="19"/>
       <c r="B26" s="3" t="s">
         <v>45</v>
@@ -1675,7 +1702,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="19"/>
       <c r="B27" s="3" t="s">
         <v>48</v>
@@ -1700,7 +1727,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="19"/>
       <c r="B28" s="3" t="s">
         <v>50</v>
@@ -1725,7 +1752,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A29" s="19"/>
       <c r="B29" s="3" t="s">
         <v>52</v>
@@ -1750,7 +1777,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A30" s="19"/>
       <c r="B30" s="3" t="s">
         <v>54</v>
@@ -1775,7 +1802,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A31" s="19"/>
       <c r="B31" s="3" t="s">
         <v>56</v>
@@ -1800,7 +1827,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A32" s="19"/>
       <c r="B32" s="3" t="s">
         <v>56</v>
@@ -1825,7 +1852,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A33" s="19"/>
       <c r="B33" s="3" t="s">
         <v>56</v>
@@ -1850,7 +1877,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A34" s="19"/>
       <c r="B34" s="3" t="s">
         <v>60</v>
@@ -1875,7 +1902,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A35" s="19"/>
       <c r="B35" s="3" t="s">
         <v>60</v>
@@ -1900,7 +1927,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A36" s="19"/>
       <c r="B36" s="3" t="s">
         <v>63</v>
@@ -1925,7 +1952,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A37" s="19"/>
       <c r="B37" s="3" t="s">
         <v>65</v>
@@ -1950,7 +1977,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="38" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A38" s="19"/>
       <c r="B38" s="3" t="s">
         <v>67</v>
@@ -1975,7 +2002,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A39" s="19"/>
       <c r="B39" s="3" t="s">
         <v>69</v>
@@ -2000,7 +2027,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="40" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A40" s="19"/>
       <c r="B40" s="3" t="s">
         <v>71</v>
@@ -2025,7 +2052,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="19"/>
       <c r="B41" s="3" t="s">
         <v>73</v>
@@ -2050,7 +2077,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A42" s="19"/>
       <c r="B42" s="3" t="s">
         <v>75</v>
@@ -2073,7 +2100,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A43" s="19"/>
       <c r="B43" s="3" t="s">
         <v>77</v>
@@ -2097,7 +2124,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A44" s="19"/>
       <c r="B44" s="3" t="s">
         <v>79</v>
@@ -2121,7 +2148,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A45" s="19"/>
       <c r="B45" s="3" t="s">
         <v>81</v>
@@ -2145,7 +2172,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A46" s="19"/>
       <c r="B46" s="3" t="s">
         <v>81</v>
@@ -2169,7 +2196,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A47" s="19"/>
       <c r="B47" s="3" t="s">
         <v>84</v>
@@ -2193,7 +2220,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A48" s="19"/>
       <c r="B48" s="3" t="s">
         <v>86</v>
@@ -2217,7 +2244,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="49" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A49" s="19"/>
       <c r="B49" s="3" t="s">
         <v>88</v>
@@ -2241,7 +2268,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A50" s="19"/>
       <c r="B50" s="3" t="s">
         <v>90</v>
@@ -2265,7 +2292,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A51" s="19"/>
       <c r="B51" s="3" t="s">
         <v>92</v>
@@ -2289,7 +2316,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A52" s="19"/>
       <c r="B52" s="6" t="s">
         <v>94</v>
@@ -2313,7 +2340,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="53" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A53" s="19"/>
       <c r="B53" s="6" t="s">
         <v>96</v>
@@ -2330,7 +2357,7 @@
       <c r="G53" s="4"/>
       <c r="H53" s="1"/>
     </row>
-    <row r="54" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A54" s="19"/>
       <c r="B54" s="6" t="s">
         <v>96</v>
@@ -2354,7 +2381,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="55" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A55" s="19"/>
       <c r="B55" s="6" t="s">
         <v>98</v>
@@ -2378,7 +2405,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="56" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A56" s="19"/>
       <c r="B56" s="6" t="s">
         <v>100</v>
@@ -2402,7 +2429,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="57" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A57" s="19"/>
       <c r="B57" s="6" t="s">
         <v>102</v>
@@ -2426,7 +2453,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="58" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A58" s="19"/>
       <c r="B58" s="6" t="s">
         <v>104</v>
@@ -2450,7 +2477,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="59" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A59" s="19"/>
       <c r="B59" s="6" t="s">
         <v>106</v>
@@ -2474,7 +2501,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="60" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A60" s="19"/>
       <c r="B60" s="6" t="s">
         <v>108</v>
@@ -2498,7 +2525,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="61" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A61" s="19"/>
       <c r="B61" s="6" t="s">
         <v>110</v>
@@ -2515,7 +2542,7 @@
       <c r="G61" s="4"/>
       <c r="H61" s="1"/>
     </row>
-    <row r="62" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A62" s="19"/>
       <c r="B62" s="6" t="s">
         <v>110</v>
@@ -2539,7 +2566,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="63" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A63" s="19"/>
       <c r="B63" s="6" t="s">
         <v>112</v>
@@ -2556,7 +2583,7 @@
       <c r="G63" s="4"/>
       <c r="H63" s="1"/>
     </row>
-    <row r="64" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A64" s="19"/>
       <c r="B64" s="6" t="s">
         <v>112</v>
@@ -2576,11 +2603,11 @@
         <v>300</v>
       </c>
       <c r="H64" s="1">
-        <f t="shared" ref="H64:H103" si="42">D64</f>
+        <f t="shared" ref="H64:H66" si="42">D64</f>
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A65" s="19"/>
       <c r="B65" s="6" t="s">
         <v>114</v>
@@ -2604,7 +2631,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="66" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A66" s="20"/>
       <c r="B66" s="6" t="s">
         <v>116</v>
@@ -2627,7 +2654,7 @@
         <v>088</v>
       </c>
     </row>
-    <row r="67" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2644,7 +2671,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="68" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2661,7 +2688,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="69" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -2678,7 +2705,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="70" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -2695,7 +2722,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="71" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -2712,7 +2739,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="72" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -2729,7 +2756,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="73" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -2746,7 +2773,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="74" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -2763,7 +2790,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="75" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -2780,7 +2807,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="76" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -2797,7 +2824,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -2814,7 +2841,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -2831,7 +2858,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="79" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -2848,7 +2875,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2865,7 +2892,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="81" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2882,7 +2909,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="82" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -2899,7 +2926,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="83" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -2916,7 +2943,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="84" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -2933,7 +2960,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="85" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -2950,7 +2977,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="86" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -2967,7 +2994,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="87" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -2984,7 +3011,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="88" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -3001,7 +3028,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="89" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -3018,7 +3045,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="90" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -3035,7 +3062,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="91" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -3052,7 +3079,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="92" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -3069,7 +3096,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -3086,7 +3113,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -3103,7 +3130,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -3120,7 +3147,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="96" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -3137,7 +3164,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -3154,7 +3181,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="98" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -3171,7 +3198,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="99" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -3188,7 +3215,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="100" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -3205,7 +3232,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="101" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -3222,7 +3249,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="102" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A102" s="1"/>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -3239,7 +3266,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="103" spans="1:8" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:8" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A103" s="1"/>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>

</xml_diff>